<commit_message>
Final Tweak (I Think)
</commit_message>
<xml_diff>
--- a/samples/templates/32readwriteScatterChart3.xlsx
+++ b/samples/templates/32readwriteScatterChart3.xlsx
@@ -562,7 +562,9 @@
             <a:pPr>
               <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="000000"/>
+                  <a:srgbClr val="000000">
+                    <a:alpha val="50000"/>
+                  </a:srgbClr>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
                 <a:ea typeface="Calibri"/>

</xml_diff>